<commit_message>
completed synopsis and rsults after receiving final data
</commit_message>
<xml_diff>
--- a/primary_outcomesQES.xlsx
+++ b/primary_outcomesQES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">UPDRS_items20_21__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">Bullock et al. 2021</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">MDS_UPDRS_III_items10_15_16_17_18__zuranolone_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">11</t>
+    <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">Choi et al. 2000</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">UPDRS_item20__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">13</t>
   </si>
   <si>
     <t xml:space="preserve">Çınar et al. 2013</t>
@@ -167,7 +167,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__apomorphine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">Dirkx et al. 2019</t>
@@ -185,7 +185,7 @@
     <t xml:space="preserve">MDS_UPDRS_III_items10_15_16_17_18__placebo_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">15</t>
+    <t xml:space="preserve">16</t>
   </si>
   <si>
     <t xml:space="preserve">Eggert et al. 2010</t>
@@ -203,7 +203,7 @@
     <t xml:space="preserve">UPDRS_items20_21__arm2_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">17</t>
+    <t xml:space="preserve">18</t>
   </si>
   <si>
     <t xml:space="preserve">Evidente et al. 2003</t>
@@ -215,13 +215,13 @@
     <t xml:space="preserve">UPDRS_III_item20__piribedil_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
+    <t xml:space="preserve">19</t>
   </si>
   <si>
     <t xml:space="preserve">Fischer et al. 1990</t>
   </si>
   <si>
-    <t xml:space="preserve">19</t>
+    <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">Frazzitta et al. 2013</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">UPDRS_items20_21__physiotherapy_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">20</t>
+    <t xml:space="preserve">21</t>
   </si>
   <si>
     <t xml:space="preserve">Friedman et al. 1997</t>
@@ -251,7 +251,7 @@
     <t xml:space="preserve">UPDRS_III_tremor_score__clozapine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
+    <t xml:space="preserve">23</t>
   </si>
   <si>
     <t xml:space="preserve">Glass (2003)</t>
@@ -263,7 +263,7 @@
     <t xml:space="preserve">UPDRS_III_item20__dihydroergocriptin_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">24</t>
+    <t xml:space="preserve">25</t>
   </si>
   <si>
     <t xml:space="preserve">Haas et al. 2006</t>
@@ -275,7 +275,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__wbv_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">25</t>
+    <t xml:space="preserve">26</t>
   </si>
   <si>
     <t xml:space="preserve">Hartelt et al. 2020</t>
@@ -287,25 +287,25 @@
     <t xml:space="preserve">UPDRS_III_items20_21__multimodal-therapy_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">27</t>
+    <t xml:space="preserve">28</t>
   </si>
   <si>
     <t xml:space="preserve">Hellmann et al. 2008</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">29</t>
   </si>
   <si>
     <t xml:space="preserve">Hiremath (2012)</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
     <t xml:space="preserve">Hughes et al. 1990</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">31</t>
   </si>
   <si>
     <t xml:space="preserve">Ikeda et al. 2015</t>
@@ -317,7 +317,7 @@
     <t xml:space="preserve">UPDRS_item16_20_21__zonisamide_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">32</t>
+    <t xml:space="preserve">33</t>
   </si>
   <si>
     <t xml:space="preserve">Jansen (1994)</t>
@@ -329,7 +329,7 @@
     <t xml:space="preserve">UPDRS_item16_20_21__clozapine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">33</t>
+    <t xml:space="preserve">34</t>
   </si>
   <si>
     <t xml:space="preserve">Jitkritsadakul et al. 2015</t>
@@ -341,31 +341,31 @@
     <t xml:space="preserve">UPDRS_items16_20__EMS_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">34</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">Jost et al. 2008</t>
   </si>
   <si>
-    <t xml:space="preserve">38</t>
+    <t xml:space="preserve">39</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987</t>
   </si>
   <si>
-    <t xml:space="preserve">39</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987.1</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
+    <t xml:space="preserve">41</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987.2</t>
   </si>
   <si>
-    <t xml:space="preserve">43</t>
+    <t xml:space="preserve">44</t>
   </si>
   <si>
     <t xml:space="preserve">Levin et al. 2010</t>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__pramipexole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">48</t>
+    <t xml:space="preserve">49</t>
   </si>
   <si>
     <t xml:space="preserve">Lotan et al. 2014</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__cannabis_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">50</t>
+    <t xml:space="preserve">51</t>
   </si>
   <si>
     <t xml:space="preserve">Maeda et al. 2015</t>
@@ -401,13 +401,13 @@
     <t xml:space="preserve">UPDRS_III_items20_21__zonisamide_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">51</t>
+    <t xml:space="preserve">52</t>
   </si>
   <si>
     <t xml:space="preserve">Mailland et al. 2011</t>
   </si>
   <si>
-    <t xml:space="preserve">53</t>
+    <t xml:space="preserve">54</t>
   </si>
   <si>
     <t xml:space="preserve">Mark et al. 1989</t>
@@ -416,31 +416,25 @@
     <t xml:space="preserve">improvements_in_UPDRS_tremor_scores_ percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">54</t>
+    <t xml:space="preserve">55</t>
   </si>
   <si>
     <t xml:space="preserve">Mentenopoulos et al. 1989</t>
   </si>
   <si>
-    <t xml:space="preserve">55</t>
+    <t xml:space="preserve">56</t>
   </si>
   <si>
     <t xml:space="preserve">Mizuno et al. 1995</t>
   </si>
   <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_baseline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPDRS_III_items20_21__pergolide-levodopa_follow-up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
+    <t xml:space="preserve">61</t>
   </si>
   <si>
     <t xml:space="preserve">Mueller et al. 2003</t>
   </si>
   <si>
-    <t xml:space="preserve">61</t>
+    <t xml:space="preserve">62</t>
   </si>
   <si>
     <t xml:space="preserve">Mueller et al. 2003.1</t>
@@ -452,7 +446,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__amantadine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">62</t>
+    <t xml:space="preserve">63</t>
   </si>
   <si>
     <t xml:space="preserve">Nakanishi et al. 1991</t>
@@ -467,19 +461,19 @@
     <t xml:space="preserve">change in disability score tremor subscore</t>
   </si>
   <si>
-    <t xml:space="preserve">75</t>
+    <t xml:space="preserve">76</t>
   </si>
   <si>
     <t xml:space="preserve">Pollok et al. 2009</t>
   </si>
   <si>
-    <t xml:space="preserve">77</t>
+    <t xml:space="preserve">78</t>
   </si>
   <si>
     <t xml:space="preserve">Rabey et al. 1994</t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
+    <t xml:space="preserve">79</t>
   </si>
   <si>
     <t xml:space="preserve">Rahimi et al. 2015</t>
@@ -491,19 +485,19 @@
     <t xml:space="preserve">UPDRS_III_item20__botulinum-toxin_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">80</t>
+    <t xml:space="preserve">81</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2002</t>
   </si>
   <si>
-    <t xml:space="preserve">81</t>
+    <t xml:space="preserve">82</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2003</t>
   </si>
   <si>
-    <t xml:space="preserve">82</t>
+    <t xml:space="preserve">83</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2005</t>
@@ -515,31 +509,31 @@
     <t xml:space="preserve">UPDRS_items16_20_21__ropinirole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">83</t>
+    <t xml:space="preserve">84</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann &amp; Jost (2010)</t>
   </si>
   <si>
-    <t xml:space="preserve">84</t>
+    <t xml:space="preserve">85</t>
   </si>
   <si>
     <t xml:space="preserve">Ridgel et al. 2012</t>
   </si>
   <si>
-    <t xml:space="preserve">85</t>
+    <t xml:space="preserve">86</t>
   </si>
   <si>
     <t xml:space="preserve">Rondot &amp; Ziegler (1992)</t>
   </si>
   <si>
-    <t xml:space="preserve">86</t>
+    <t xml:space="preserve">87</t>
   </si>
   <si>
     <t xml:space="preserve">Saavedra-Escalona et al. 2005</t>
   </si>
   <si>
-    <t xml:space="preserve">87</t>
+    <t xml:space="preserve">88</t>
   </si>
   <si>
     <t xml:space="preserve">Sahoo et al. 2020</t>
@@ -557,7 +551,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">88</t>
+    <t xml:space="preserve">89</t>
   </si>
   <si>
     <t xml:space="preserve">Samotus et al. 2017</t>
@@ -569,31 +563,31 @@
     <t xml:space="preserve">UPDRS_III_item20__incobotulinumtoxin_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">89</t>
+    <t xml:space="preserve">90</t>
   </si>
   <si>
     <t xml:space="preserve">Samotus et al. 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">90</t>
+    <t xml:space="preserve">91</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009</t>
   </si>
   <si>
-    <t xml:space="preserve">91</t>
+    <t xml:space="preserve">92</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009.1</t>
   </si>
   <si>
-    <t xml:space="preserve">92</t>
+    <t xml:space="preserve">93</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009.2</t>
   </si>
   <si>
-    <t xml:space="preserve">95</t>
+    <t xml:space="preserve">96</t>
   </si>
   <si>
     <t xml:space="preserve">Schrag et al. 1999</t>
@@ -605,13 +599,13 @@
     <t xml:space="preserve">UPDRS_III_items20_21__biperiden_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">100</t>
+    <t xml:space="preserve">101</t>
   </si>
   <si>
     <t xml:space="preserve">Spieker et al. 1995</t>
   </si>
   <si>
-    <t xml:space="preserve">103</t>
+    <t xml:space="preserve">104</t>
   </si>
   <si>
     <t xml:space="preserve">Takahashi et al. 2008</t>
@@ -623,19 +617,19 @@
     <t xml:space="preserve">UPDRS_II_item16__pramipexole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">105</t>
+    <t xml:space="preserve">106</t>
   </si>
   <si>
     <t xml:space="preserve">Trosch et al. 1994</t>
   </si>
   <si>
-    <t xml:space="preserve">106</t>
+    <t xml:space="preserve">107</t>
   </si>
   <si>
     <t xml:space="preserve">Van Laar et al. 1998</t>
   </si>
   <si>
-    <t xml:space="preserve">108</t>
+    <t xml:space="preserve">109</t>
   </si>
   <si>
     <t xml:space="preserve">Weiner et al. 1989</t>
@@ -647,7 +641,7 @@
     <t xml:space="preserve">UPDRS_item20__PHNO_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">109</t>
+    <t xml:space="preserve">110</t>
   </si>
   <si>
     <t xml:space="preserve">Wilken et al. 2019</t>
@@ -659,19 +653,19 @@
     <t xml:space="preserve">MDS_UPDRS_III_item15_16_17_18__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">110</t>
+    <t xml:space="preserve">111</t>
   </si>
   <si>
     <t xml:space="preserve">Yoshii et al. 1996</t>
   </si>
   <si>
-    <t xml:space="preserve">111</t>
+    <t xml:space="preserve">112</t>
   </si>
   <si>
     <t xml:space="preserve">Zach et al. 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">112</t>
+    <t xml:space="preserve">113</t>
   </si>
   <si>
     <t xml:space="preserve">Zach et al. 2020</t>
@@ -683,7 +677,7 @@
     <t xml:space="preserve">MDS_UPDRS_item17_18__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">117</t>
+    <t xml:space="preserve">118</t>
   </si>
   <si>
     <t xml:space="preserve">Ziegler M.  &amp; Rondot P. (1999)</t>
@@ -1831,12 +1825,8 @@
       <c r="E36" t="s">
         <v>22</v>
       </c>
-      <c r="F36" t="s">
-        <v>138</v>
-      </c>
-      <c r="G36" t="s">
-        <v>139</v>
-      </c>
+      <c r="F36"/>
+      <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
@@ -1844,10 +1834,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C37" t="s">
         <v>13</v>
@@ -1863,19 +1853,19 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s">
         <v>142</v>
       </c>
-      <c r="B38" t="s">
+      <c r="E38" t="s">
         <v>143</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38" t="s">
-        <v>145</v>
       </c>
       <c r="F38"/>
       <c r="G38"/>
@@ -1886,19 +1876,19 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
         <v>146</v>
       </c>
-      <c r="B39" t="s">
+      <c r="E39" t="s">
         <v>147</v>
-      </c>
-      <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" t="s">
-        <v>148</v>
-      </c>
-      <c r="E39" t="s">
-        <v>149</v>
       </c>
       <c r="F39"/>
       <c r="G39"/>
@@ -1906,15 +1896,15 @@
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C40" t="s">
         <v>13</v>
@@ -1930,10 +1920,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C41" t="s">
         <v>13</v>
@@ -1949,19 +1939,19 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
         <v>155</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>156</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>157</v>
-      </c>
-      <c r="E42" t="s">
-        <v>158</v>
       </c>
       <c r="F42"/>
       <c r="G42"/>
@@ -1972,10 +1962,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
@@ -1991,10 +1981,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
         <v>13</v>
@@ -2010,19 +2000,19 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45" t="s">
         <v>163</v>
       </c>
-      <c r="B45" t="s">
+      <c r="E45" t="s">
         <v>164</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" t="s">
-        <v>165</v>
-      </c>
-      <c r="E45" t="s">
-        <v>166</v>
       </c>
       <c r="F45"/>
       <c r="G45"/>
@@ -2033,10 +2023,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
         <v>13</v>
@@ -2052,10 +2042,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -2071,10 +2061,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B48" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
@@ -2090,10 +2080,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
@@ -2109,25 +2099,25 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s">
         <v>175</v>
       </c>
-      <c r="B50" t="s">
+      <c r="E50" t="s">
         <v>176</v>
       </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>177</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>178</v>
-      </c>
-      <c r="F50" t="s">
-        <v>179</v>
-      </c>
-      <c r="G50" t="s">
-        <v>180</v>
       </c>
       <c r="H50"/>
       <c r="I50"/>
@@ -2136,19 +2126,19 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
         <v>181</v>
       </c>
-      <c r="B51" t="s">
+      <c r="E51" t="s">
         <v>182</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>183</v>
-      </c>
-      <c r="E51" t="s">
-        <v>184</v>
       </c>
       <c r="F51"/>
       <c r="G51"/>
@@ -2159,10 +2149,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B52" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C52" t="s">
         <v>13</v>
@@ -2178,10 +2168,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B53" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C53" t="s">
         <v>13</v>
@@ -2197,10 +2187,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B54" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C54" t="s">
         <v>13</v>
@@ -2216,10 +2206,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -2235,10 +2225,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B56" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C56" t="s">
         <v>13</v>
@@ -2250,10 +2240,10 @@
         <v>50</v>
       </c>
       <c r="F56" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G56" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H56"/>
       <c r="I56"/>
@@ -2262,10 +2252,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B57" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C57" t="s">
         <v>13</v>
@@ -2281,19 +2271,19 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" t="s">
+        <v>198</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" t="s">
         <v>199</v>
       </c>
-      <c r="B58" t="s">
+      <c r="E58" t="s">
         <v>200</v>
-      </c>
-      <c r="C58" t="s">
-        <v>13</v>
-      </c>
-      <c r="D58" t="s">
-        <v>201</v>
-      </c>
-      <c r="E58" t="s">
-        <v>202</v>
       </c>
       <c r="F58"/>
       <c r="G58"/>
@@ -2304,10 +2294,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B59" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C59" t="s">
         <v>13</v>
@@ -2323,10 +2313,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B60" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C60" t="s">
         <v>13</v>
@@ -2342,19 +2332,19 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>205</v>
+      </c>
+      <c r="B61" t="s">
+        <v>206</v>
+      </c>
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61" t="s">
         <v>207</v>
       </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
         <v>208</v>
-      </c>
-      <c r="C61" t="s">
-        <v>13</v>
-      </c>
-      <c r="D61" t="s">
-        <v>209</v>
-      </c>
-      <c r="E61" t="s">
-        <v>210</v>
       </c>
       <c r="F61"/>
       <c r="G61"/>
@@ -2365,19 +2355,19 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>209</v>
+      </c>
+      <c r="B62" t="s">
+        <v>210</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" t="s">
         <v>211</v>
       </c>
-      <c r="B62" t="s">
+      <c r="E62" t="s">
         <v>212</v>
-      </c>
-      <c r="C62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
-        <v>213</v>
-      </c>
-      <c r="E62" t="s">
-        <v>214</v>
       </c>
       <c r="F62"/>
       <c r="G62"/>
@@ -2388,10 +2378,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B63" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C63" t="s">
         <v>13</v>
@@ -2407,10 +2397,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B64" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C64" t="s">
         <v>13</v>
@@ -2426,19 +2416,19 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" t="s">
+        <v>218</v>
+      </c>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" t="s">
         <v>219</v>
       </c>
-      <c r="B65" t="s">
+      <c r="E65" t="s">
         <v>220</v>
-      </c>
-      <c r="C65" t="s">
-        <v>13</v>
-      </c>
-      <c r="D65" t="s">
-        <v>221</v>
-      </c>
-      <c r="E65" t="s">
-        <v>222</v>
       </c>
       <c r="F65"/>
       <c r="G65"/>
@@ -2449,10 +2439,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B66" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C66" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
improved analyses and pipeline for automatic plotting of results
</commit_message>
<xml_diff>
--- a/primary_outcomesQES.xlsx
+++ b/primary_outcomesQES.xlsx
@@ -287,25 +287,25 @@
     <t xml:space="preserve">UPDRS_III_items20_21__multimodal-therapy_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">28</t>
+    <t xml:space="preserve">29</t>
   </si>
   <si>
     <t xml:space="preserve">Hellmann et al. 2008</t>
   </si>
   <si>
-    <t xml:space="preserve">29</t>
+    <t xml:space="preserve">30</t>
   </si>
   <si>
     <t xml:space="preserve">Hiremath (2012)</t>
   </si>
   <si>
-    <t xml:space="preserve">30</t>
+    <t xml:space="preserve">31</t>
   </si>
   <si>
     <t xml:space="preserve">Hughes et al. 1990</t>
   </si>
   <si>
-    <t xml:space="preserve">31</t>
+    <t xml:space="preserve">32</t>
   </si>
   <si>
     <t xml:space="preserve">Ikeda et al. 2015</t>
@@ -317,7 +317,7 @@
     <t xml:space="preserve">UPDRS_item16_20_21__zonisamide_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">33</t>
+    <t xml:space="preserve">34</t>
   </si>
   <si>
     <t xml:space="preserve">Jansen (1994)</t>
@@ -329,7 +329,7 @@
     <t xml:space="preserve">UPDRS_item16_20_21__clozapine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">34</t>
+    <t xml:space="preserve">35</t>
   </si>
   <si>
     <t xml:space="preserve">Jitkritsadakul et al. 2015</t>
@@ -341,31 +341,31 @@
     <t xml:space="preserve">UPDRS_items16_20__EMS_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">35</t>
+    <t xml:space="preserve">36</t>
   </si>
   <si>
     <t xml:space="preserve">Jost et al. 2008</t>
   </si>
   <si>
-    <t xml:space="preserve">39</t>
+    <t xml:space="preserve">40</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
+    <t xml:space="preserve">41</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987.1</t>
   </si>
   <si>
-    <t xml:space="preserve">41</t>
+    <t xml:space="preserve">42</t>
   </si>
   <si>
     <t xml:space="preserve">Koller et al. 1987.2</t>
   </si>
   <si>
-    <t xml:space="preserve">44</t>
+    <t xml:space="preserve">45</t>
   </si>
   <si>
     <t xml:space="preserve">Levin et al. 2010</t>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__pramipexole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">49</t>
+    <t xml:space="preserve">50</t>
   </si>
   <si>
     <t xml:space="preserve">Lotan et al. 2014</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__cannabis_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">51</t>
+    <t xml:space="preserve">52</t>
   </si>
   <si>
     <t xml:space="preserve">Maeda et al. 2015</t>
@@ -401,13 +401,13 @@
     <t xml:space="preserve">UPDRS_III_items20_21__zonisamide_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">52</t>
+    <t xml:space="preserve">53</t>
   </si>
   <si>
     <t xml:space="preserve">Mailland et al. 2011</t>
   </si>
   <si>
-    <t xml:space="preserve">54</t>
+    <t xml:space="preserve">55</t>
   </si>
   <si>
     <t xml:space="preserve">Mark et al. 1989</t>
@@ -416,25 +416,25 @@
     <t xml:space="preserve">improvements_in_UPDRS_tremor_scores_ percentage</t>
   </si>
   <si>
-    <t xml:space="preserve">55</t>
+    <t xml:space="preserve">56</t>
   </si>
   <si>
     <t xml:space="preserve">Mentenopoulos et al. 1989</t>
   </si>
   <si>
-    <t xml:space="preserve">56</t>
+    <t xml:space="preserve">57</t>
   </si>
   <si>
     <t xml:space="preserve">Mizuno et al. 1995</t>
   </si>
   <si>
-    <t xml:space="preserve">61</t>
+    <t xml:space="preserve">62</t>
   </si>
   <si>
     <t xml:space="preserve">Mueller et al. 2003</t>
   </si>
   <si>
-    <t xml:space="preserve">62</t>
+    <t xml:space="preserve">63</t>
   </si>
   <si>
     <t xml:space="preserve">Mueller et al. 2003.1</t>
@@ -446,7 +446,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__amantadine_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">63</t>
+    <t xml:space="preserve">64</t>
   </si>
   <si>
     <t xml:space="preserve">Nakanishi et al. 1991</t>
@@ -461,19 +461,19 @@
     <t xml:space="preserve">change in disability score tremor subscore</t>
   </si>
   <si>
-    <t xml:space="preserve">76</t>
+    <t xml:space="preserve">77</t>
   </si>
   <si>
     <t xml:space="preserve">Pollok et al. 2009</t>
   </si>
   <si>
-    <t xml:space="preserve">78</t>
+    <t xml:space="preserve">79</t>
   </si>
   <si>
     <t xml:space="preserve">Rabey et al. 1994</t>
   </si>
   <si>
-    <t xml:space="preserve">79</t>
+    <t xml:space="preserve">80</t>
   </si>
   <si>
     <t xml:space="preserve">Rahimi et al. 2015</t>
@@ -485,19 +485,19 @@
     <t xml:space="preserve">UPDRS_III_item20__botulinum-toxin_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">81</t>
+    <t xml:space="preserve">82</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2002</t>
   </si>
   <si>
-    <t xml:space="preserve">82</t>
+    <t xml:space="preserve">83</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2003</t>
   </si>
   <si>
-    <t xml:space="preserve">83</t>
+    <t xml:space="preserve">84</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann et al. 2005</t>
@@ -509,31 +509,31 @@
     <t xml:space="preserve">UPDRS_items16_20_21__ropinirole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">84</t>
+    <t xml:space="preserve">85</t>
   </si>
   <si>
     <t xml:space="preserve">Reichmann &amp; Jost (2010)</t>
   </si>
   <si>
-    <t xml:space="preserve">85</t>
+    <t xml:space="preserve">86</t>
   </si>
   <si>
     <t xml:space="preserve">Ridgel et al. 2012</t>
   </si>
   <si>
-    <t xml:space="preserve">86</t>
+    <t xml:space="preserve">87</t>
   </si>
   <si>
     <t xml:space="preserve">Rondot &amp; Ziegler (1992)</t>
   </si>
   <si>
-    <t xml:space="preserve">87</t>
+    <t xml:space="preserve">88</t>
   </si>
   <si>
     <t xml:space="preserve">Saavedra-Escalona et al. 2005</t>
   </si>
   <si>
-    <t xml:space="preserve">88</t>
+    <t xml:space="preserve">89</t>
   </si>
   <si>
     <t xml:space="preserve">Sahoo et al. 2020</t>
@@ -551,7 +551,7 @@
     <t xml:space="preserve">UPDRS_III_items20_21__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">89</t>
+    <t xml:space="preserve">90</t>
   </si>
   <si>
     <t xml:space="preserve">Samotus et al. 2017</t>
@@ -563,31 +563,31 @@
     <t xml:space="preserve">UPDRS_III_item20__incobotulinumtoxin_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">90</t>
+    <t xml:space="preserve">91</t>
   </si>
   <si>
     <t xml:space="preserve">Samotus et al. 2020</t>
   </si>
   <si>
-    <t xml:space="preserve">91</t>
+    <t xml:space="preserve">92</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009</t>
   </si>
   <si>
-    <t xml:space="preserve">92</t>
+    <t xml:space="preserve">93</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009.1</t>
   </si>
   <si>
-    <t xml:space="preserve">93</t>
+    <t xml:space="preserve">94</t>
   </si>
   <si>
     <t xml:space="preserve">Schlesinger et al. 2009.2</t>
   </si>
   <si>
-    <t xml:space="preserve">96</t>
+    <t xml:space="preserve">97</t>
   </si>
   <si>
     <t xml:space="preserve">Schrag et al. 1999</t>
@@ -599,13 +599,13 @@
     <t xml:space="preserve">UPDRS_III_items20_21__biperiden_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">101</t>
+    <t xml:space="preserve">102</t>
   </si>
   <si>
     <t xml:space="preserve">Spieker et al. 1995</t>
   </si>
   <si>
-    <t xml:space="preserve">104</t>
+    <t xml:space="preserve">105</t>
   </si>
   <si>
     <t xml:space="preserve">Takahashi et al. 2008</t>
@@ -617,19 +617,19 @@
     <t xml:space="preserve">UPDRS_II_item16__pramipexole_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">106</t>
+    <t xml:space="preserve">107</t>
   </si>
   <si>
     <t xml:space="preserve">Trosch et al. 1994</t>
   </si>
   <si>
-    <t xml:space="preserve">107</t>
+    <t xml:space="preserve">108</t>
   </si>
   <si>
     <t xml:space="preserve">Van Laar et al. 1998</t>
   </si>
   <si>
-    <t xml:space="preserve">109</t>
+    <t xml:space="preserve">110</t>
   </si>
   <si>
     <t xml:space="preserve">Weiner et al. 1989</t>
@@ -641,7 +641,7 @@
     <t xml:space="preserve">UPDRS_item20__PHNO_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">110</t>
+    <t xml:space="preserve">111</t>
   </si>
   <si>
     <t xml:space="preserve">Wilken et al. 2019</t>
@@ -653,19 +653,19 @@
     <t xml:space="preserve">MDS_UPDRS_III_item15_16_17_18__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">111</t>
+    <t xml:space="preserve">112</t>
   </si>
   <si>
     <t xml:space="preserve">Yoshii et al. 1996</t>
   </si>
   <si>
-    <t xml:space="preserve">112</t>
+    <t xml:space="preserve">113</t>
   </si>
   <si>
     <t xml:space="preserve">Zach et al. 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">113</t>
+    <t xml:space="preserve">114</t>
   </si>
   <si>
     <t xml:space="preserve">Zach et al. 2020</t>
@@ -677,7 +677,7 @@
     <t xml:space="preserve">MDS_UPDRS_item17_18__levodopa_follow-up</t>
   </si>
   <si>
-    <t xml:space="preserve">118</t>
+    <t xml:space="preserve">119</t>
   </si>
   <si>
     <t xml:space="preserve">Ziegler M.  &amp; Rondot P. (1999)</t>

</xml_diff>

<commit_message>
tidies up code for analyses and continued with manuscript
</commit_message>
<xml_diff>
--- a/primary_outcomesQES.xlsx
+++ b/primary_outcomesQES.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t xml:space="preserve">change in disability score tremor subscore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nigro et al. 2019</t>
   </si>
   <si>
     <t xml:space="preserve">77</t>
@@ -1909,10 +1915,18 @@
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" t="s">
+        <v>28</v>
+      </c>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -1947,12 +1961,8 @@
       <c r="C42" t="s">
         <v>13</v>
       </c>
-      <c r="D42" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" t="s">
-        <v>156</v>
-      </c>
+      <c r="D42"/>
+      <c r="E42"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -1962,16 +1972,20 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
         <v>157</v>
       </c>
-      <c r="B43" t="s">
+      <c r="E43" t="s">
         <v>158</v>
       </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43"/>
-      <c r="E43"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2008,12 +2022,8 @@
       <c r="C45" t="s">
         <v>13</v>
       </c>
-      <c r="D45" t="s">
-        <v>163</v>
-      </c>
-      <c r="E45" t="s">
-        <v>164</v>
-      </c>
+      <c r="D45"/>
+      <c r="E45"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2023,16 +2033,20 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>163</v>
+      </c>
+      <c r="B46" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
         <v>165</v>
       </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
         <v>166</v>
       </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46"/>
-      <c r="E46"/>
       <c r="F46"/>
       <c r="G46"/>
       <c r="H46"/>
@@ -2107,18 +2121,10 @@
       <c r="C50" t="s">
         <v>13</v>
       </c>
-      <c r="D50" t="s">
-        <v>175</v>
-      </c>
-      <c r="E50" t="s">
-        <v>176</v>
-      </c>
-      <c r="F50" t="s">
-        <v>177</v>
-      </c>
-      <c r="G50" t="s">
-        <v>178</v>
-      </c>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
@@ -2126,22 +2132,26 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C51" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>177</v>
+      </c>
+      <c r="E51" t="s">
+        <v>178</v>
+      </c>
+      <c r="F51" t="s">
         <v>179</v>
       </c>
-      <c r="B51" t="s">
+      <c r="G51" t="s">
         <v>180</v>
       </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>181</v>
-      </c>
-      <c r="E51" t="s">
-        <v>182</v>
-      </c>
-      <c r="F51"/>
-      <c r="G51"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
@@ -2149,16 +2159,20 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" t="s">
+        <v>182</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
         <v>183</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" t="s">
         <v>184</v>
       </c>
-      <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52"/>
-      <c r="E52"/>
       <c r="F52"/>
       <c r="G52"/>
       <c r="H52"/>
@@ -2233,18 +2247,10 @@
       <c r="C56" t="s">
         <v>13</v>
       </c>
-      <c r="D56" t="s">
-        <v>49</v>
-      </c>
-      <c r="E56" t="s">
-        <v>50</v>
-      </c>
-      <c r="F56" t="s">
-        <v>193</v>
-      </c>
-      <c r="G56" t="s">
-        <v>194</v>
-      </c>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
@@ -2252,18 +2258,26 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" t="s">
+        <v>13</v>
+      </c>
+      <c r="D57" t="s">
+        <v>49</v>
+      </c>
+      <c r="E57" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" t="s">
         <v>195</v>
       </c>
-      <c r="B57" t="s">
+      <c r="G57" t="s">
         <v>196</v>
       </c>
-      <c r="C57" t="s">
-        <v>13</v>
-      </c>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
@@ -2279,12 +2293,8 @@
       <c r="C58" t="s">
         <v>13</v>
       </c>
-      <c r="D58" t="s">
-        <v>199</v>
-      </c>
-      <c r="E58" t="s">
-        <v>200</v>
-      </c>
+      <c r="D58"/>
+      <c r="E58"/>
       <c r="F58"/>
       <c r="G58"/>
       <c r="H58"/>
@@ -2294,16 +2304,20 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>199</v>
+      </c>
+      <c r="B59" t="s">
+        <v>200</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
         <v>201</v>
       </c>
-      <c r="B59" t="s">
+      <c r="E59" t="s">
         <v>202</v>
       </c>
-      <c r="C59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D59"/>
-      <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
       <c r="H59"/>
@@ -2340,12 +2354,8 @@
       <c r="C61" t="s">
         <v>13</v>
       </c>
-      <c r="D61" t="s">
-        <v>207</v>
-      </c>
-      <c r="E61" t="s">
-        <v>208</v>
-      </c>
+      <c r="D61"/>
+      <c r="E61"/>
       <c r="F61"/>
       <c r="G61"/>
       <c r="H61"/>
@@ -2355,19 +2365,19 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" t="s">
+        <v>208</v>
+      </c>
+      <c r="C62" t="s">
+        <v>13</v>
+      </c>
+      <c r="D62" t="s">
         <v>209</v>
       </c>
-      <c r="B62" t="s">
+      <c r="E62" t="s">
         <v>210</v>
-      </c>
-      <c r="C62" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
-        <v>211</v>
-      </c>
-      <c r="E62" t="s">
-        <v>212</v>
       </c>
       <c r="F62"/>
       <c r="G62"/>
@@ -2378,16 +2388,20 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>211</v>
+      </c>
+      <c r="B63" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" t="s">
+        <v>13</v>
+      </c>
+      <c r="D63" t="s">
         <v>213</v>
       </c>
-      <c r="B63" t="s">
+      <c r="E63" t="s">
         <v>214</v>
       </c>
-      <c r="C63" t="s">
-        <v>13</v>
-      </c>
-      <c r="D63"/>
-      <c r="E63"/>
       <c r="F63"/>
       <c r="G63"/>
       <c r="H63"/>
@@ -2424,12 +2438,8 @@
       <c r="C65" t="s">
         <v>13</v>
       </c>
-      <c r="D65" t="s">
-        <v>219</v>
-      </c>
-      <c r="E65" t="s">
-        <v>220</v>
-      </c>
+      <c r="D65"/>
+      <c r="E65"/>
       <c r="F65"/>
       <c r="G65"/>
       <c r="H65"/>
@@ -2439,16 +2449,20 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B66" t="s">
+        <v>220</v>
+      </c>
+      <c r="C66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66" t="s">
         <v>221</v>
       </c>
-      <c r="B66" t="s">
+      <c r="E66" t="s">
         <v>222</v>
       </c>
-      <c r="C66" t="s">
-        <v>13</v>
-      </c>
-      <c r="D66"/>
-      <c r="E66"/>
       <c r="F66"/>
       <c r="G66"/>
       <c r="H66"/>
@@ -2456,6 +2470,25 @@
       <c r="J66"/>
       <c r="K66"/>
     </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>223</v>
+      </c>
+      <c r="B67" t="s">
+        <v>224</v>
+      </c>
+      <c r="C67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67"/>
+      <c r="E67"/>
+      <c r="F67"/>
+      <c r="G67"/>
+      <c r="H67"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="K67"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>